<commit_message>
update shopping cart & login
</commit_message>
<xml_diff>
--- a/dataExcel/datax (1).xlsx
+++ b/dataExcel/datax (1).xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="109">
   <si>
     <t>Id</t>
   </si>
@@ -349,12 +349,18 @@
   </si>
   <si>
     <t>sppk</t>
+  </si>
+  <si>
+    <t>CreatDate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -396,11 +402,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,20 +756,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="41.21875" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -776,11 +786,14 @@
       <c r="E1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -796,11 +809,14 @@
       <c r="E2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4">
+        <v>37592</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -816,11 +832,14 @@
       <c r="E3" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4">
+        <v>38029</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -836,11 +855,14 @@
       <c r="E4" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4">
+        <v>37021</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -856,11 +878,14 @@
       <c r="E5" t="b">
         <v>1</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4">
+        <v>36621</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -876,11 +901,14 @@
       <c r="E6" t="b">
         <v>1</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4">
+        <v>36960</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -896,11 +924,14 @@
       <c r="E7" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4">
+        <v>37326</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -916,11 +947,14 @@
       <c r="E8" t="b">
         <v>1</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="4">
+        <v>37633</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -936,11 +970,14 @@
       <c r="E9" t="b">
         <v>1</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="4">
+        <v>38056</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -956,11 +993,14 @@
       <c r="E10" t="b">
         <v>1</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="4">
+        <v>38634</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -976,11 +1016,14 @@
       <c r="E11" t="b">
         <v>1</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="4">
+        <v>38787</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -996,11 +1039,14 @@
       <c r="E12" t="b">
         <v>1</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="4">
+        <v>39212</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1016,11 +1062,14 @@
       <c r="E13" t="b">
         <v>1</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="4">
+        <v>39632</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1036,11 +1085,14 @@
       <c r="E14" t="b">
         <v>1</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="4">
+        <v>39875</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1056,11 +1108,14 @@
       <c r="E15" t="b">
         <v>1</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="4">
+        <v>40369</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1076,11 +1131,14 @@
       <c r="E16" t="b">
         <v>1</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="4">
+        <v>36979</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1096,11 +1154,14 @@
       <c r="E17" t="b">
         <v>1</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="4">
+        <v>40704</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1116,11 +1177,14 @@
       <c r="E18" t="b">
         <v>1</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="4">
+        <v>38903</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1136,11 +1200,14 @@
       <c r="E19" t="b">
         <v>1</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="4">
+        <v>41155</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1156,11 +1223,14 @@
       <c r="E20" t="b">
         <v>1</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="4">
+        <v>40612</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1176,11 +1246,14 @@
       <c r="E21" t="b">
         <v>1</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="4">
+        <v>37262</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1196,11 +1269,14 @@
       <c r="E22" t="b">
         <v>1</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="4">
+        <v>39423</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1216,11 +1292,14 @@
       <c r="E23" t="b">
         <v>1</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="4">
+        <v>40947</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1236,11 +1315,14 @@
       <c r="E24" t="b">
         <v>1</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="4">
+        <v>41681</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1256,11 +1338,14 @@
       <c r="E25" t="b">
         <v>1</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="4">
+        <v>44321</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1276,11 +1361,14 @@
       <c r="E26" t="b">
         <v>1</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="4">
+        <v>38238</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1296,11 +1384,14 @@
       <c r="E27" t="b">
         <v>1</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="4">
+        <v>40211</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1316,11 +1407,14 @@
       <c r="E28" t="b">
         <v>1</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="4">
+        <v>38787</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1336,11 +1430,14 @@
       <c r="E29" t="b">
         <v>1</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="4">
+        <v>39880</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1356,11 +1453,14 @@
       <c r="E30" t="b">
         <v>1</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="4">
+        <v>39817</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1376,11 +1476,14 @@
       <c r="E31" t="b">
         <v>1</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="4">
+        <v>44682</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1396,11 +1499,14 @@
       <c r="E32" t="b">
         <v>1</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="4">
+        <v>44502</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1416,11 +1522,14 @@
       <c r="E33" t="b">
         <v>1</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="4">
+        <v>44745</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1436,11 +1545,14 @@
       <c r="E34" t="b">
         <v>1</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="4">
+        <v>44442</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1456,11 +1568,14 @@
       <c r="E35" t="b">
         <v>1</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="4">
+        <v>44661</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1476,11 +1591,14 @@
       <c r="E36" t="b">
         <v>1</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="4">
+        <v>44449</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1496,11 +1614,14 @@
       <c r="E37" t="b">
         <v>1</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="4">
+        <v>44480</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1516,11 +1637,14 @@
       <c r="E38" t="b">
         <v>1</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="4">
+        <v>44537</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1536,11 +1660,14 @@
       <c r="E39" t="b">
         <v>1</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="4">
+        <v>44478</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1556,11 +1683,14 @@
       <c r="E40" t="b">
         <v>1</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F40" s="4">
+        <v>44389</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1576,11 +1706,14 @@
       <c r="E41" t="b">
         <v>1</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F41" s="4">
+        <v>44296</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1596,11 +1729,14 @@
       <c r="E42" t="b">
         <v>1</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F42" s="4">
+        <v>44267</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1616,11 +1752,14 @@
       <c r="E43" t="b">
         <v>1</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F43" s="4">
+        <v>44236</v>
+      </c>
+      <c r="G43" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1636,11 +1775,14 @@
       <c r="E44" t="b">
         <v>1</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F44" s="4">
+        <v>44199</v>
+      </c>
+      <c r="G44" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1656,11 +1798,14 @@
       <c r="E45" t="b">
         <v>1</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="F45" s="4">
+        <v>44411</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1676,11 +1821,14 @@
       <c r="E46" t="b">
         <v>1</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F46" s="4">
+        <v>44540</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1696,7 +1844,10 @@
       <c r="E47" t="b">
         <v>1</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F47" s="4">
+        <v>44298</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>